<commit_message>
restructuring big data file w/ ppfd for each study, extracting additional ppfd's from studies with a range measured, and updated raw folder files
</commit_message>
<xml_diff>
--- a/extraction/raw extraction/sancho1997/sancho1997.xlsx
+++ b/extraction/raw extraction/sancho1997/sancho1997.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/margaretslein/lichen/extraction/raw extraction/sancho1997/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9E11FA9-EF54-9F47-8D85-FC0959E1393D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4612595-5DA9-5E48-A04A-2D80185C6322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30420" yWindow="-8700" windowWidth="22780" windowHeight="16720" xr2:uid="{38E3F4B7-2944-1E46-AD3C-CD9309D25C62}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="13">
   <si>
     <t>x</t>
   </si>
@@ -64,6 +64,15 @@
   </si>
   <si>
     <t>freyi</t>
+  </si>
+  <si>
+    <t>60-70</t>
+  </si>
+  <si>
+    <t>220-240</t>
+  </si>
+  <si>
+    <t>610-650</t>
   </si>
 </sst>
 </file>
@@ -416,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668AA1D3-1DD6-8445-8DFC-82BBF949DA5C}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E25"/>
+      <selection activeCell="J12" sqref="H1:J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,410 +452,1226 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0.111856823266219</v>
+        <v>0.30922448979591599</v>
       </c>
       <c r="B2">
-        <v>3.4399999999999902</v>
+        <v>-0.73371428571428599</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
-        <v>5</v>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>5.2013422818791897</v>
+        <v>7.3070204081632602</v>
       </c>
       <c r="B3">
-        <v>5.9799999999999898</v>
+        <v>-1.22742857142857</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>5</v>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>10.2908277404921</v>
+        <v>14.377877551020401</v>
       </c>
       <c r="B4">
-        <v>5.96</v>
+        <v>-1.3554285714285701</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
-        <v>5</v>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>15.1565995525727</v>
+        <v>21.300408163265299</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>-2.7085714285714202</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
-        <v>5</v>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>20.3020134228187</v>
+        <v>28.367510204081601</v>
       </c>
       <c r="B6">
-        <v>5.8999999999999897</v>
+        <v>-3.6777142857142802</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
-        <v>5</v>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>25.223713646532399</v>
+        <v>35.363755102040798</v>
       </c>
       <c r="B7">
-        <v>4.4800000000000004</v>
+        <v>-4.51885714285714</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
-      <c r="E7" t="s">
-        <v>5</v>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>0.16778523489933</v>
+        <v>0.24955102040815899</v>
       </c>
       <c r="B8">
-        <v>-0.72000000000000197</v>
+        <v>1.8994285714285699</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>5.1454138702460801</v>
+        <v>7.3237551020408098</v>
       </c>
       <c r="B9">
-        <v>-1.24</v>
+        <v>2.5211428571428498</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>10.234899328858999</v>
+        <v>14.322040816326499</v>
       </c>
       <c r="B10">
-        <v>-1.36</v>
+        <v>2.1371428571428499</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>15.212527964205799</v>
+        <v>21.2473469387755</v>
       </c>
       <c r="B11">
-        <v>-2.7</v>
+        <v>1.4057142857142799</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>20.246085011185599</v>
+        <v>28.3884081632653</v>
       </c>
       <c r="B12">
-        <v>-3.68</v>
+        <v>1.00342857142857</v>
       </c>
       <c r="C12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>25.2796420581655</v>
+        <v>35.3841632653061</v>
       </c>
       <c r="B13">
-        <v>-4.5199999999999996</v>
+        <v>5.2571428571429303E-2</v>
       </c>
       <c r="C13" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>-0.15035377358490301</v>
+        <v>0.179346938775506</v>
       </c>
       <c r="B14">
-        <v>5.1094339622641503</v>
+        <v>2.1737142857142802</v>
       </c>
       <c r="C14" t="s">
         <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>4.97627470799641</v>
+        <v>7.3282448979591797</v>
       </c>
       <c r="B15">
-        <v>7.20251572327044</v>
+        <v>3.52685714285714</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>9.8860062893081793</v>
+        <v>14.324653061224399</v>
       </c>
       <c r="B16">
-        <v>7.4842767295597401</v>
+        <v>2.72228571428571</v>
       </c>
       <c r="C16" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E16">
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>14.8007917789757</v>
+        <v>21.394204081632601</v>
       </c>
       <c r="B17">
-        <v>6.3169811320754699</v>
+        <v>2.3017142857142798</v>
       </c>
       <c r="C17" t="s">
         <v>7</v>
       </c>
       <c r="D17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E17">
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>19.9344395777178</v>
+        <v>28.461632653061201</v>
       </c>
       <c r="B18">
-        <v>6.3974842767295499</v>
+        <v>1.4057142857142799</v>
       </c>
       <c r="C18" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>24.850488544474299</v>
+        <v>35.244408163265298</v>
       </c>
       <c r="B19">
-        <v>4.8679245283018799</v>
+        <v>0.747428571428569</v>
       </c>
       <c r="C19" t="s">
         <v>7</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>-0.12789195867026101</v>
+        <v>0.180163265306124</v>
       </c>
       <c r="B20">
-        <v>-1.3308176100628899</v>
+        <v>2.3565714285714199</v>
       </c>
       <c r="C20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D20" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>4.8968160377358503</v>
+        <v>7.3317551020408098</v>
       </c>
       <c r="B21">
-        <v>-2.0150943396226402</v>
+        <v>4.3131428571428501</v>
       </c>
       <c r="C21" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D21" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>9.9199797843665802</v>
+        <v>14.333224489795899</v>
       </c>
       <c r="B22">
-        <v>-2.2566037735848998</v>
+        <v>4.6422857142857099</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D22" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>14.946232030548</v>
+        <v>21.400979591836698</v>
       </c>
       <c r="B23">
-        <v>-3.3836477987421301</v>
+        <v>3.8194285714285701</v>
       </c>
       <c r="C23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D23" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>19.860455974842701</v>
+        <v>28.330367346938701</v>
       </c>
       <c r="B24">
-        <v>-4.3899371069182296</v>
+        <v>4.0022857142857102</v>
       </c>
       <c r="C24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D24" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>24.9983153638814</v>
+        <v>35.612734693877499</v>
       </c>
       <c r="B25">
-        <v>-5.51698113207547</v>
+        <v>3.2525714285714198</v>
       </c>
       <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>0.32783673469387797</v>
+      </c>
+      <c r="B26">
+        <v>3.4354285714285702</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>7.3391836734693801</v>
+      </c>
+      <c r="B27">
+        <v>5.9771428571428498</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>14.4819591836734</v>
+      </c>
+      <c r="B28">
+        <v>5.9588571428571404</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>6</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>21.410775510204001</v>
+      </c>
+      <c r="B29">
+        <v>6.01371428571428</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>28.481714285714201</v>
+      </c>
+      <c r="B30">
+        <v>5.9039999999999999</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>35.332489795918299</v>
+      </c>
+      <c r="B31">
+        <v>4.4777142857142804</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>0.33077551020407298</v>
+      </c>
+      <c r="B32">
+        <v>4.0937142857142801</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>7.3414693877550903</v>
+      </c>
+      <c r="B33">
+        <v>6.4891428571428502</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>14.424081632652999</v>
+      </c>
+      <c r="B34">
+        <v>8.9942857142857093</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>21.274775510204002</v>
+      </c>
+      <c r="B35">
+        <v>7.5497142857142796</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>28.419265306122401</v>
+      </c>
+      <c r="B36">
+        <v>7.9154285714285697</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>35.413959183673398</v>
+      </c>
+      <c r="B37">
+        <v>6.7268571428571402</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>-0.14285714285715301</v>
+      </c>
+      <c r="B38">
+        <v>-1.32336018411967</v>
+      </c>
+      <c r="C38" t="s">
         <v>8</v>
       </c>
-      <c r="D25" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>6.8571428571428399</v>
+      </c>
+      <c r="B39">
+        <v>-2.0230149597238198</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>13.857142857142801</v>
+      </c>
+      <c r="B40">
+        <v>-2.24395857307249</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>20.928571428571399</v>
+      </c>
+      <c r="B41">
+        <v>-3.3670886075949298</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>27.857142857142801</v>
+      </c>
+      <c r="B42">
+        <v>-4.3797468354430302</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>34.928571428571402</v>
+      </c>
+      <c r="B43">
+        <v>-5.5397008055235899</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>-0.21428571428572199</v>
+      </c>
+      <c r="B44">
+        <v>2.4879171461449898</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>6.8571428571428399</v>
+      </c>
+      <c r="B45">
+        <v>2.9850402761795101</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
+        <v>13.857142857142801</v>
+      </c>
+      <c r="B46">
+        <v>1.8434982738780199</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>20.785714285714199</v>
+      </c>
+      <c r="B47">
+        <v>1.5489067894131201</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>27.928571428571399</v>
+      </c>
+      <c r="B48">
+        <v>0.86766398158803204</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>34.928571428571402</v>
+      </c>
+      <c r="B49">
+        <v>-0.531645569620254</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>-0.28571428571429103</v>
+      </c>
+      <c r="B50">
+        <v>3.1691599539700799</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>6.8571428571428399</v>
+      </c>
+      <c r="B51">
+        <v>4.64211737629459</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>13.857142857142801</v>
+      </c>
+      <c r="B52">
+        <v>2.1012658227848</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>20.857142857142801</v>
+      </c>
+      <c r="B53">
+        <v>2.39585730724971</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>28.071428571428498</v>
+      </c>
+      <c r="B54">
+        <v>1.9723820483314101</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>34.857142857142797</v>
+      </c>
+      <c r="B55">
+        <v>0.66513233601841204</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>-0.14285714285715301</v>
+      </c>
+      <c r="B56">
+        <v>3.7583429228998799</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>6.9285714285714102</v>
+      </c>
+      <c r="B57">
+        <v>6.1150747986190996</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>14.1428571428571</v>
+      </c>
+      <c r="B58">
+        <v>4.3107019562715703</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>20.857142857142801</v>
+      </c>
+      <c r="B59">
+        <v>3.8688147295742201</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>27.857142857142801</v>
+      </c>
+      <c r="B60">
+        <v>3.6478711162255402</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>35.142857142857103</v>
+      </c>
+      <c r="B61">
+        <v>1.40161104718066</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>-0.14285714285715301</v>
+      </c>
+      <c r="B62">
+        <v>5.0840046029919401</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>6.8571428571428399</v>
+      </c>
+      <c r="B63">
+        <v>7.2197928653624803</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>13.9285714285714</v>
+      </c>
+      <c r="B64">
+        <v>7.47756041426927</v>
+      </c>
+      <c r="C64" t="s">
+        <v>7</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>20.785714285714199</v>
+      </c>
+      <c r="B65">
+        <v>6.3360184119677703</v>
+      </c>
+      <c r="C65" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>27.928571428571399</v>
+      </c>
+      <c r="B66">
+        <v>6.4096662830840003</v>
+      </c>
+      <c r="C66" t="s">
+        <v>7</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>34.857142857142797</v>
+      </c>
+      <c r="B67">
+        <v>4.8630609896432597</v>
+      </c>
+      <c r="C67" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>-0.14285714285715301</v>
+      </c>
+      <c r="B68">
+        <v>5.9309551208285303</v>
+      </c>
+      <c r="C68" t="s">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>6.8571428571428399</v>
+      </c>
+      <c r="B69">
+        <v>8.9505178365937805</v>
+      </c>
+      <c r="C69" t="s">
+        <v>7</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>13.857142857142801</v>
+      </c>
+      <c r="B70">
+        <v>9.7422324510932103</v>
+      </c>
+      <c r="C70" t="s">
+        <v>7</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>20.785714285714199</v>
+      </c>
+      <c r="B71">
+        <v>10.1657077100115</v>
+      </c>
+      <c r="C71" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>27.928571428571399</v>
+      </c>
+      <c r="B72">
+        <v>8.8400460299194403</v>
+      </c>
+      <c r="C72" t="s">
+        <v>7</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>35.142857142857103</v>
+      </c>
+      <c r="B73">
+        <v>7.4039125431530497</v>
+      </c>
+      <c r="C73" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>